<commit_message>
Fix template file rewrite error.
</commit_message>
<xml_diff>
--- a/spec/fixtures/simple_template.xlsx
+++ b/spec/fixtures/simple_template.xlsx
@@ -20,13 +20,13 @@
     <t>Some template</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>It's a Replaced placeholder 1</t>
-  </si>
-  <si>
-    <t>It's a Replaced placeholder 2</t>
+    <t>${PLACEHOLDER_3}</t>
+  </si>
+  <si>
+    <t>It's a ${PLACEHOLDER_1}</t>
+  </si>
+  <si>
+    <t>It's a ${PLACEHOLDER_2}</t>
   </si>
 </sst>
 </file>
@@ -41,6 +41,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -63,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -129,7 +131,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -213,7 +215,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Processing of placeholder inline formatting.
</commit_message>
<xml_diff>
--- a/spec/fixtures/simple_template.xlsx
+++ b/spec/fixtures/simple_template.xlsx
@@ -26,7 +26,28 @@
     <t>It's a ${PLACEHOLDER_1}</t>
   </si>
   <si>
-    <t>It's a ${PLACEHOLDER_2}</t>
+    <r>
+      <t xml:space="preserve">It's a ${</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PLACEHOLDER_2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -36,7 +57,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -61,6 +82,13 @@
     <font>
       <b val="true"/>
       <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -210,12 +238,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -258,8 +287,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Inserting images into the generated document
</commit_message>
<xml_diff>
--- a/spec/fixtures/simple_template.xlsx
+++ b/spec/fixtures/simple_template.xlsx
@@ -5,17 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Some template</t>
   </si>
@@ -23,11 +28,20 @@
     <t>${PLACEHOLDER_3}</t>
   </si>
   <si>
+    <t>${IMAGE:300x700}</t>
+  </si>
+  <si>
     <t>It's a ${PLACEHOLDER_1}</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">It's a ${</t>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>It's a ${</t>
     </r>
     <r>
       <rPr>
@@ -37,7 +51,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">PLACEHOLDER_2</t>
+      <t>PLACEHOLDER_2</t>
     </r>
     <r>
       <rPr>
@@ -46,7 +60,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">}</t>
+      <t>}</t>
     </r>
   </si>
 </sst>
@@ -238,21 +252,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -267,14 +281,19 @@
         <v>#VALUE!</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J10" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -287,8 +306,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Страница &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix rendering document without  images.
</commit_message>
<xml_diff>
--- a/spec/fixtures/simple_template.xlsx
+++ b/spec/fixtures/simple_template.xlsx
@@ -28,7 +28,7 @@
     <t>${PLACEHOLDER_3}</t>
   </si>
   <si>
-    <t>${IMAGE:300x700}</t>
+    <t>${IMAGE:200x300}</t>
   </si>
   <si>
     <t>It's a ${PLACEHOLDER_1}</t>
@@ -258,15 +258,15 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix rendering document with multiple images.
</commit_message>
<xml_diff>
--- a/spec/fixtures/simple_template.xlsx
+++ b/spec/fixtures/simple_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Some template</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>It's a ${PLACEHOLDER_1}</t>
+  </si>
+  <si>
+    <t>${IMAGE:100x200}</t>
+  </si>
+  <si>
+    <t>${IMAGE2:200x300}</t>
   </si>
   <si>
     <r>
@@ -258,15 +264,13 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.1377551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,9 +295,19 @@
         <v>3</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>

</xml_diff>